<commit_message>
fix: change in the company html
</commit_message>
<xml_diff>
--- a/src/assets/modelo_crear_clientes.xlsx
+++ b/src/assets/modelo_crear_clientes.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27514"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="415" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD6A6924-D1DF-4638-9356-0F18B7F8321D}"/>
+  <xr:revisionPtr revIDLastSave="417" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A4BDEE0-FCF1-47CA-890A-EEE1D70F5576}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Nombre</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>Condición ante el IVA</t>
   </si>
   <si>
@@ -99,7 +96,7 @@
     <t>Descuento</t>
   </si>
   <si>
-    <t>limite_de_credito</t>
+    <t>Limite de Credito</t>
   </si>
   <si>
     <t>CP</t>
@@ -481,33 +478,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:X6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" customWidth="1"/>
-    <col min="13" max="13" width="12" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" customWidth="1"/>
-    <col min="16" max="16" width="40.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" customWidth="1"/>
-    <col min="23" max="23" width="16.7109375" customWidth="1"/>
-    <col min="24" max="24" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" customWidth="1"/>
+    <col min="12" max="12" width="12" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="15" width="40.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,19 +538,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
@@ -565,10 +562,10 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
       <c r="V1" t="s">
@@ -576,31 +573,28 @@
       </c>
       <c r="W1" t="s">
         <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 P1 E1:F1" xr:uid="{CA05FF94-1CA6-4651-B269-18A98151BE01}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{FB104F44-931B-4C7C-8311-5380F102AE19}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 O1 D1:E1" xr:uid="{CA05FF94-1CA6-4651-B269-18A98151BE01}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{FB104F44-931B-4C7C-8311-5380F102AE19}">
       <formula1>"DNI, CUIL"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{F6DE02A6-5ECA-4775-8899-F8093B7003E0}">
       <formula1>"Cliente, Proveedor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{02FA8122-2939-4C2B-B75F-E3E55B5F1A96}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{02FA8122-2939-4C2B-B75F-E3E55B5F1A96}">
       <formula1>"Responsable Inscripto, Responsable No Inscripto, Exento, Consumidor Final, Monotributista  "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576" xr:uid="{67AB1A50-2A30-42D8-9C50-73F682025473}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{67AB1A50-2A30-42D8-9C50-73F682025473}">
       <formula1>"Si, No"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{C06AE3AD-4581-4D65-8C84-CD531F30A36A}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{C06AE3AD-4581-4D65-8C84-CD531F30A36A}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{437216C3-F683-4149-92FB-7C7F47B7EFA9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{437216C3-F683-4149-92FB-7C7F47B7EFA9}">
       <formula1>"Hombre, Mujer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix: change in the structure of excel
</commit_message>
<xml_diff>
--- a/src/assets/modelo_crear_clientes.xlsx
+++ b/src/assets/modelo_crear_clientes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27514"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="417" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A4BDEE0-FCF1-47CA-890A-EEE1D70F5576}"/>
+  <xr:revisionPtr revIDLastSave="545" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C4FF6B4-CA71-432D-AFE5-74C6E282286A}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -57,49 +57,43 @@
     <t>Dirección</t>
   </si>
   <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Piso</t>
+  </si>
+  <si>
+    <t>Dpto</t>
+  </si>
+  <si>
+    <t>Código postal</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Provincia</t>
+  </si>
+  <si>
     <t>Ciudad</t>
   </si>
   <si>
     <t>Teléfono</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>Mails</t>
+  </si>
+  <si>
+    <t>Género</t>
   </si>
   <si>
     <t>Cumpleaños</t>
   </si>
   <si>
-    <t>Género</t>
-  </si>
-  <si>
-    <t>Observación</t>
-  </si>
-  <si>
-    <t>Habilitado para comprar en cuenta corriente</t>
-  </si>
-  <si>
-    <t>Piso</t>
-  </si>
-  <si>
-    <t>Dpto</t>
-  </si>
-  <si>
-    <t>Número</t>
-  </si>
-  <si>
-    <t>Latitud</t>
-  </si>
-  <si>
-    <t>Longitud</t>
-  </si>
-  <si>
-    <t>Descuento</t>
+    <t>habilitado para cuenta corriente</t>
   </si>
   <si>
     <t>Limite de Credito</t>
-  </si>
-  <si>
-    <t>CP</t>
   </si>
 </sst>
 </file>
@@ -156,13 +150,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -478,14 +474,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="5" width="20.28515625" customWidth="1"/>
@@ -493,18 +490,19 @@
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="28.140625" customWidth="1"/>
-    <col min="12" max="12" width="12" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="3" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" customWidth="1"/>
-    <col min="15" max="15" width="40.5703125" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
     <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="27.85546875" customWidth="1"/>
     <col min="18" max="18" width="19.5703125" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="3" customWidth="1"/>
+    <col min="20" max="20" width="30" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +557,7 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -568,16 +566,20 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="G2" s="4"/>
+      <c r="Q2" s="5"/>
+      <c r="U2" s="4"/>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="G3" s="4"/>
+      <c r="Q3" s="5"/>
+      <c r="U3" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 O1 D1:E1" xr:uid="{CA05FF94-1CA6-4651-B269-18A98151BE01}"/>
+  <dataValidations count="9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1 C1:E1 O1:O1048576 R1 T1 M1 N1" xr:uid="{CA05FF94-1CA6-4651-B269-18A98151BE01}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{FB104F44-931B-4C7C-8311-5380F102AE19}">
       <formula1>"DNI, CUIL"</formula1>
     </dataValidation>
@@ -587,15 +589,21 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{02FA8122-2939-4C2B-B75F-E3E55B5F1A96}">
       <formula1>"Responsable Inscripto, Responsable No Inscripto, Exento, Consumidor Final, Monotributista  "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{67AB1A50-2A30-42D8-9C50-73F682025473}">
-      <formula1>"Si, No"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{C06AE3AD-4581-4D65-8C84-CD531F30A36A}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{C06AE3AD-4581-4D65-8C84-CD531F30A36A}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{437216C3-F683-4149-92FB-7C7F47B7EFA9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576" xr:uid="{54E217E0-4507-4065-8A74-628BB556AD02}">
       <formula1>"Hombre, Mujer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576" xr:uid="{27E786D1-B609-4EB5-9643-1BECB91760F3}">
+      <formula1>"Si, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{55F2CB51-F35A-4E22-8713-5D0B19C31498}">
+      <formula1>"Argentina"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576" xr:uid="{2E278F67-2F74-420B-A530-42869593D01F}">
+      <formula1>"Buenos Aires, Córdoba, Santa Fe, San Luis, Mendoza, Jujuy, Salta, Tucuman, Santigo Del Estero, La Pamoa, Chaco  "</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>